<commit_message>
Fix the validation issue with Normalization planning template destination container coord.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Normalization_planning_v4_7_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Normalization_planning_v4_7_0.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>UFG</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -13479,7 +13479,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I1000" type="list">
-      <formula1>IF($K6="384-well plate",Index!$H$2:$H$385,IF($K6="96-well plate", Index!$F$2:$F$97, ""))</formula1>
+      <formula1>IF($K6="384-well plate",Index!$H$2:$H$385,IF($K6="96-well plate", Index!$F$2:$F$97, Index!$H$2:$H$385))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>